<commit_message>
Uploading the three puzzle results
</commit_message>
<xml_diff>
--- a/Reports/Thesis/results/Pomeranz 805 Piece Puzzle Results.xlsx
+++ b/Reports/Thesis/results/Pomeranz 805 Piece Puzzle Results.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27960" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27960" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="One Puzzle" sheetId="3" r:id="rId1"/>
     <sheet name="Two Puzzles" sheetId="4" r:id="rId2"/>
+    <sheet name="Three Puzzles" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="81">
   <si>
     <t>Solver Type</t>
   </si>
@@ -240,6 +241,24 @@
   </si>
   <si>
     <t>pomeranz_805_6 | pomeranz_805_11</t>
+  </si>
+  <si>
+    <t>pomeranz_805_10 | pomeranz_805_12</t>
+  </si>
+  <si>
+    <t>Solved Puzzle #3</t>
+  </si>
+  <si>
+    <t>pomeranz_805_17 | pomeranz_805_19 | pomeranz_805_3</t>
+  </si>
+  <si>
+    <t>Solved Puzzle #4</t>
+  </si>
+  <si>
+    <t>Solved Puzzle#4</t>
+  </si>
+  <si>
+    <t>Input Puzzle #2</t>
   </si>
 </sst>
 </file>
@@ -1143,7 +1162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -4666,10 +4685,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW47"/>
+  <dimension ref="A1:AW49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AX2" sqref="AX2"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="AR48" sqref="A48:AR48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -4942,7 +4961,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="3">
-        <f>D3-E3</f>
+        <f t="shared" ref="F3:F47" si="0">D3-E3</f>
         <v>0</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -5089,7 +5108,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="4">
-        <f>D4-E4</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -5236,7 +5255,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="4">
-        <f>D5-E5</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -5383,7 +5402,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="3">
-        <f>D6-E6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -5530,7 +5549,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="3">
-        <f>D7-E7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -5677,7 +5696,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="3">
-        <f>D8-E8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -5824,7 +5843,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="3">
-        <f>D9-E9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G9" s="3" t="s">
@@ -5971,7 +5990,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="4">
-        <f>D10-E10</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="G10" s="4" t="s">
@@ -6118,7 +6137,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="3">
-        <f>D11-E11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -6265,7 +6284,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="3">
-        <f>D12-E12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -6412,7 +6431,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="3">
-        <f>D13-E13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G13" s="3" t="s">
@@ -6559,7 +6578,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="3">
-        <f>D14-E14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -6706,7 +6725,7 @@
         <v>2</v>
       </c>
       <c r="F15" s="3">
-        <f>D15-E15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -6853,7 +6872,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="3">
-        <f>D16-E16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G16" s="3" t="s">
@@ -7000,7 +7019,7 @@
         <v>2</v>
       </c>
       <c r="F17" s="3">
-        <f>D17-E17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -7147,7 +7166,7 @@
         <v>2</v>
       </c>
       <c r="F18" s="3">
-        <f>D18-E18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -7294,7 +7313,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="3">
-        <f>D19-E19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -7441,7 +7460,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="3">
-        <f>D20-E20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -7588,7 +7607,7 @@
         <v>2</v>
       </c>
       <c r="F21" s="3">
-        <f>D21-E21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G21" s="3" t="s">
@@ -7735,7 +7754,7 @@
         <v>2</v>
       </c>
       <c r="F22" s="3">
-        <f>D22-E22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -7882,7 +7901,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="3">
-        <f>D23-E23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G23" s="3" t="s">
@@ -8029,7 +8048,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="3">
-        <f>D24-E24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G24" s="3" t="s">
@@ -8176,7 +8195,7 @@
         <v>2</v>
       </c>
       <c r="F25" s="5">
-        <f>D25-E25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G25" s="5" t="s">
@@ -8323,7 +8342,7 @@
         <v>2</v>
       </c>
       <c r="F26" s="3">
-        <f>D26-E26</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G26" s="3" t="s">
@@ -8470,7 +8489,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="3">
-        <f>D27-E27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G27" s="3" t="s">
@@ -8617,7 +8636,7 @@
         <v>2</v>
       </c>
       <c r="F28" s="3">
-        <f>D28-E28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G28" s="3" t="s">
@@ -8764,7 +8783,7 @@
         <v>2</v>
       </c>
       <c r="F29" s="3">
-        <f>D29-E29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G29" s="3" t="s">
@@ -8911,7 +8930,7 @@
         <v>2</v>
       </c>
       <c r="F30" s="3">
-        <f>D30-E30</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G30" s="3" t="s">
@@ -9058,7 +9077,7 @@
         <v>2</v>
       </c>
       <c r="F31" s="3">
-        <f>D31-E31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G31" s="3" t="s">
@@ -9205,7 +9224,7 @@
         <v>2</v>
       </c>
       <c r="F32" s="3">
-        <f>D32-E32</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G32" s="3" t="s">
@@ -9352,7 +9371,7 @@
         <v>2</v>
       </c>
       <c r="F33" s="3">
-        <f>D33-E33</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G33" s="3" t="s">
@@ -9499,7 +9518,7 @@
         <v>2</v>
       </c>
       <c r="F34" s="3">
-        <f>D34-E34</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G34" s="3" t="s">
@@ -9646,7 +9665,7 @@
         <v>2</v>
       </c>
       <c r="F35" s="3">
-        <f>D35-E35</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G35" s="3" t="s">
@@ -9793,7 +9812,7 @@
         <v>2</v>
       </c>
       <c r="F36" s="3">
-        <f>D36-E36</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G36" s="3" t="s">
@@ -9940,7 +9959,7 @@
         <v>2</v>
       </c>
       <c r="F37" s="3">
-        <f>D37-E37</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G37" s="3" t="s">
@@ -10087,7 +10106,7 @@
         <v>2</v>
       </c>
       <c r="F38" s="3">
-        <f>D38-E38</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G38" s="3" t="s">
@@ -10234,7 +10253,7 @@
         <v>2</v>
       </c>
       <c r="F39" s="3">
-        <f>D39-E39</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G39" s="3" t="s">
@@ -10381,7 +10400,7 @@
         <v>2</v>
       </c>
       <c r="F40" s="3">
-        <f>D40-E40</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G40" s="3" t="s">
@@ -10528,7 +10547,7 @@
         <v>2</v>
       </c>
       <c r="F41" s="3">
-        <f>D41-E41</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G41" s="3" t="s">
@@ -10675,7 +10694,7 @@
         <v>2</v>
       </c>
       <c r="F42" s="3">
-        <f>D42-E42</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G42" s="3" t="s">
@@ -10822,7 +10841,7 @@
         <v>2</v>
       </c>
       <c r="F43" s="3">
-        <f>D43-E43</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G43" s="3" t="s">
@@ -10969,7 +10988,7 @@
         <v>2</v>
       </c>
       <c r="F44" s="3">
-        <f>D44-E44</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G44" s="3" t="s">
@@ -11116,7 +11135,7 @@
         <v>2</v>
       </c>
       <c r="F45" s="3">
-        <f>D45-E45</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G45" s="3" t="s">
@@ -11263,7 +11282,7 @@
         <v>2</v>
       </c>
       <c r="F46" s="3">
-        <f>D46-E46</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G46" s="3" t="s">
@@ -11410,7 +11429,7 @@
         <v>2</v>
       </c>
       <c r="F47" s="3">
-        <f>D47-E47</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G47" s="3" t="s">
@@ -11538,6 +11557,298 @@
       </c>
       <c r="AV47" s="3">
         <v>3164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="4">
+        <v>2</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D48" s="4">
+        <v>2</v>
+      </c>
+      <c r="E48" s="4">
+        <v>5</v>
+      </c>
+      <c r="F48" s="4">
+        <v>-3</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H48" s="4">
+        <v>805</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J48" s="4">
+        <v>808</v>
+      </c>
+      <c r="K48" s="4">
+        <v>0.68316831683199997</v>
+      </c>
+      <c r="L48" s="4">
+        <v>3.7128712871299999E-3</v>
+      </c>
+      <c r="M48" s="4">
+        <v>0</v>
+      </c>
+      <c r="N48" s="4">
+        <v>0</v>
+      </c>
+      <c r="O48" s="4">
+        <v>253</v>
+      </c>
+      <c r="P48" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q48" s="4">
+        <v>808</v>
+      </c>
+      <c r="R48" s="4">
+        <v>0.68316831683199997</v>
+      </c>
+      <c r="S48" s="4">
+        <v>3.7128712871299999E-3</v>
+      </c>
+      <c r="T48" s="4">
+        <v>0</v>
+      </c>
+      <c r="U48" s="4">
+        <v>0</v>
+      </c>
+      <c r="V48" s="4">
+        <v>253</v>
+      </c>
+      <c r="W48" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="X48" s="4">
+        <v>564</v>
+      </c>
+      <c r="Y48" s="4">
+        <v>0.661872705018</v>
+      </c>
+      <c r="Z48" s="4">
+        <v>253</v>
+      </c>
+      <c r="AA48" s="4">
+        <v>12</v>
+      </c>
+      <c r="AB48" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC48" s="4">
+        <v>805</v>
+      </c>
+      <c r="AD48" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE48" s="4">
+        <v>805</v>
+      </c>
+      <c r="AF48" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG48" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH48" s="4">
+        <v>0.43354037267099998</v>
+      </c>
+      <c r="AI48" s="4">
+        <v>1.2422360248399999E-3</v>
+      </c>
+      <c r="AJ48" s="4">
+        <v>455</v>
+      </c>
+      <c r="AK48" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL48" s="4">
+        <v>805</v>
+      </c>
+      <c r="AM48" s="4">
+        <v>3.7267080745299998E-3</v>
+      </c>
+      <c r="AN48" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO48" s="4">
+        <v>0.43105590062100002</v>
+      </c>
+      <c r="AP48" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ48" s="4">
+        <v>455</v>
+      </c>
+      <c r="AR48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS48" s="8">
+        <v>321</v>
+      </c>
+      <c r="AT48" s="8">
+        <v>0.32049689441000001</v>
+      </c>
+      <c r="AU48" s="8">
+        <v>484</v>
+      </c>
+      <c r="AV48" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="3">
+        <v>2</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D49" s="3">
+        <v>2</v>
+      </c>
+      <c r="E49" s="3">
+        <v>2</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H49" s="3">
+        <v>805</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J49" s="3">
+        <v>999</v>
+      </c>
+      <c r="K49" s="3">
+        <v>0</v>
+      </c>
+      <c r="L49" s="3">
+        <v>0.194194194194</v>
+      </c>
+      <c r="M49" s="3">
+        <v>0.80580580580600003</v>
+      </c>
+      <c r="N49" s="3">
+        <v>0</v>
+      </c>
+      <c r="O49" s="3">
+        <v>0</v>
+      </c>
+      <c r="P49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q49" s="3">
+        <v>999</v>
+      </c>
+      <c r="R49" s="3">
+        <v>0.80580580580600003</v>
+      </c>
+      <c r="S49" s="3">
+        <v>0.194194194194</v>
+      </c>
+      <c r="T49" s="3">
+        <v>0</v>
+      </c>
+      <c r="U49" s="3">
+        <v>0</v>
+      </c>
+      <c r="V49" s="3">
+        <v>0</v>
+      </c>
+      <c r="W49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X49" s="3">
+        <v>1581</v>
+      </c>
+      <c r="Y49" s="3">
+        <v>0.50474383301699999</v>
+      </c>
+      <c r="Z49" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA49" s="3">
+        <v>776</v>
+      </c>
+      <c r="AB49" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC49" s="3">
+        <v>805</v>
+      </c>
+      <c r="AD49" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE49" s="3">
+        <v>805</v>
+      </c>
+      <c r="AF49" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG49" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH49" s="3">
+        <v>0.75900621118</v>
+      </c>
+      <c r="AI49" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ49" s="3">
+        <v>194</v>
+      </c>
+      <c r="AK49" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL49" s="3">
+        <v>805</v>
+      </c>
+      <c r="AM49" s="3">
+        <v>0.46459627329199998</v>
+      </c>
+      <c r="AN49" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO49" s="3">
+        <v>0.29316770186300001</v>
+      </c>
+      <c r="AP49" s="3">
+        <v>1.2422360248399999E-3</v>
+      </c>
+      <c r="AQ49" s="3">
+        <v>194</v>
+      </c>
+      <c r="AR49" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS49" s="8">
+        <v>611</v>
+      </c>
+      <c r="AT49" s="8">
+        <v>0.51956521739100003</v>
+      </c>
+      <c r="AU49" s="8">
+        <v>194</v>
+      </c>
+      <c r="AV49" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -11557,4 +11868,807 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BR4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="9" style="8"/>
+    <col min="3" max="3" width="46.25" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="13.25" style="8" customWidth="1"/>
+    <col min="6" max="6" width="21.875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="21.875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="15.25" style="8" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="13" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="15.25" style="8" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="9.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="20" width="12.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="11.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="12.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="15.625" style="8" customWidth="1"/>
+    <col min="24" max="24" width="12.25" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="17.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.75" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="15.875" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="21.875" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="14.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="15.25" style="8" customWidth="1"/>
+    <col min="31" max="31" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="34" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="37" max="37" width="15.25" style="8" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="39" max="39" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="41" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="42" max="42" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="43" max="43" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="44" max="44" width="15.625" style="8" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="46" max="46" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="48" max="48" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="49" max="49" width="15.625" style="8" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="12.25" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="51" max="51" width="17.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.75" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="53" max="53" width="15.875" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="54" max="54" width="21.875" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="55" max="55" width="14.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="56" max="56" width="15.25" style="8" customWidth="1"/>
+    <col min="57" max="57" width="14.125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="58" max="58" width="9.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="60" width="12.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="61" max="61" width="11.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="12.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="63" max="63" width="15.25" style="8" customWidth="1"/>
+    <col min="64" max="64" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="65" max="65" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="67" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="69" max="69" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="70" max="70" width="9" style="8" collapsed="1"/>
+    <col min="71" max="16384" width="9" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="D1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="I1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AD1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
+      <c r="AK1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL1" s="10"/>
+      <c r="AM1" s="10"/>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="10"/>
+      <c r="AP1" s="10"/>
+      <c r="AQ1" s="10"/>
+      <c r="AR1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="11"/>
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AX1" s="11"/>
+      <c r="AY1" s="11"/>
+      <c r="AZ1" s="11"/>
+      <c r="BA1" s="11"/>
+      <c r="BD1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="BE1" s="10"/>
+      <c r="BF1" s="10"/>
+      <c r="BG1" s="10"/>
+      <c r="BH1" s="10"/>
+      <c r="BI1" s="10"/>
+      <c r="BJ1" s="10"/>
+      <c r="BK1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="BL1" s="10"/>
+      <c r="BM1" s="10"/>
+      <c r="BN1" s="10"/>
+      <c r="BO1" s="10"/>
+      <c r="BP1" s="10"/>
+      <c r="BQ1" s="10"/>
+    </row>
+    <row r="2" spans="1:69" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BH2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="BK2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="BL2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="BM2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="BN2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BO2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BP2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BQ2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:69" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5">
+        <v>6</v>
+      </c>
+      <c r="F3" s="5">
+        <v>-3</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="5">
+        <v>805</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="5">
+        <v>805</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0.52670807453400004</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
+        <v>2.4844720496900001E-3</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5">
+        <v>379</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>805</v>
+      </c>
+      <c r="R3" s="5">
+        <v>0.52670807453400004</v>
+      </c>
+      <c r="S3" s="5">
+        <v>0</v>
+      </c>
+      <c r="T3" s="5">
+        <v>2.4844720496900001E-3</v>
+      </c>
+      <c r="U3" s="5">
+        <v>0</v>
+      </c>
+      <c r="V3" s="5">
+        <v>379</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="X3" s="5">
+        <v>426</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>0.50683229813700004</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>379</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE3" s="5">
+        <v>822</v>
+      </c>
+      <c r="AF3" s="5">
+        <v>0.97931873479300002</v>
+      </c>
+      <c r="AG3" s="5">
+        <v>2.0681265206800001E-2</v>
+      </c>
+      <c r="AH3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL3" s="5">
+        <v>822</v>
+      </c>
+      <c r="AM3" s="5">
+        <v>0.97931873479300002</v>
+      </c>
+      <c r="AN3" s="5">
+        <v>2.0681265206800001E-2</v>
+      </c>
+      <c r="AO3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS3" s="5">
+        <v>873</v>
+      </c>
+      <c r="AT3" s="5">
+        <v>0.92124856815599998</v>
+      </c>
+      <c r="AU3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="5">
+        <v>68</v>
+      </c>
+      <c r="AW3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX3" s="5">
+        <v>805</v>
+      </c>
+      <c r="AY3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AZ3" s="5">
+        <v>805</v>
+      </c>
+      <c r="BA3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC3" s="5">
+        <v>0.73788819875800005</v>
+      </c>
+      <c r="BD3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BE3" s="5">
+        <v>211</v>
+      </c>
+      <c r="BF3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="BG3" s="5">
+        <v>805</v>
+      </c>
+      <c r="BH3" s="5">
+        <v>0.52795031055899999</v>
+      </c>
+      <c r="BI3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BJ3" s="5">
+        <v>0.209937888199</v>
+      </c>
+      <c r="BK3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BL3" s="5">
+        <v>847</v>
+      </c>
+      <c r="BM3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BN3" s="5">
+        <v>4.9586776999999999E-2</v>
+      </c>
+      <c r="BO3" s="5">
+        <v>0.92325855999999995</v>
+      </c>
+      <c r="BP3" s="5">
+        <v>1.1806379999999999E-3</v>
+      </c>
+      <c r="BQ3" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:69" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="5">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="5">
+        <v>805</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="5">
+        <v>1609</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.49968924797999997</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0.50031075201999997</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>1609</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0.46239900559399999</v>
+      </c>
+      <c r="S4" s="5">
+        <v>0.49968924797999997</v>
+      </c>
+      <c r="T4" s="5">
+        <v>3.7290242386600003E-2</v>
+      </c>
+      <c r="U4" s="5">
+        <v>6.2150403977600003E-4</v>
+      </c>
+      <c r="V4" s="5">
+        <v>0</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X4" s="5">
+        <v>4021</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>0.19292464561100001</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>3216</v>
+      </c>
+      <c r="AB4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC4" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE4" s="5">
+        <v>1610</v>
+      </c>
+      <c r="AF4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AH4" s="5">
+        <v>0.49937888198800001</v>
+      </c>
+      <c r="AI4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="5">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL4" s="5">
+        <v>1610</v>
+      </c>
+      <c r="AM4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AO4" s="5">
+        <v>0.49937888198800001</v>
+      </c>
+      <c r="AP4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="5">
+        <v>1</v>
+      </c>
+      <c r="AR4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS4" s="5">
+        <v>4024</v>
+      </c>
+      <c r="AT4" s="5">
+        <v>0.196956521739</v>
+      </c>
+      <c r="AU4" s="5">
+        <v>1</v>
+      </c>
+      <c r="AV4" s="5">
+        <v>3220</v>
+      </c>
+      <c r="AW4" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX4" s="5">
+        <v>805</v>
+      </c>
+      <c r="AY4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AZ4" s="5">
+        <v>805</v>
+      </c>
+      <c r="BA4" s="5">
+        <v>6.3354037267099997E-2</v>
+      </c>
+      <c r="BB4" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC4" s="5">
+        <v>5.3416149068300001E-2</v>
+      </c>
+      <c r="BD4" s="5">
+        <v>0</v>
+      </c>
+      <c r="BE4" s="5">
+        <v>711</v>
+      </c>
+      <c r="BF4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="BG4" s="5">
+        <v>806</v>
+      </c>
+      <c r="BH4" s="5">
+        <v>0.524813895782</v>
+      </c>
+      <c r="BI4" s="5">
+        <v>1.24069478908E-3</v>
+      </c>
+      <c r="BJ4" s="5">
+        <v>0.35607940446699998</v>
+      </c>
+      <c r="BK4" s="5">
+        <v>1.24069478908E-3</v>
+      </c>
+      <c r="BL4" s="5">
+        <v>838</v>
+      </c>
+      <c r="BM4" s="5">
+        <v>1.9093078999999999E-2</v>
+      </c>
+      <c r="BN4" s="5">
+        <v>3.9379474999999997E-2</v>
+      </c>
+      <c r="BO4" s="5">
+        <v>0.754176611</v>
+      </c>
+      <c r="BP4" s="5">
+        <v>1.1933169999999999E-3</v>
+      </c>
+      <c r="BQ4" s="5">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="AR1:AV1"/>
+    <mergeCell ref="AW1:BA1"/>
+    <mergeCell ref="BD1:BJ1"/>
+    <mergeCell ref="BK1:BQ1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AD1:AJ1"/>
+    <mergeCell ref="AK1:AQ1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating the data spreadsheet to include best buddy information.
</commit_message>
<xml_diff>
--- a/Reports/Thesis/results/Pomeranz 805 Piece Puzzle Results.xlsx
+++ b/Reports/Thesis/results/Pomeranz 805 Piece Puzzle Results.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="480" yWindow="105" windowWidth="27960" windowHeight="12600"/>
   </bookViews>
   <sheets>
-    <sheet name="One Puzzle" sheetId="3" r:id="rId1"/>
-    <sheet name="Two Puzzles" sheetId="4" r:id="rId2"/>
-    <sheet name="Three Puzzles" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
+    <sheet name="One Puzzle" sheetId="3" r:id="rId2"/>
+    <sheet name="Two Puzzles" sheetId="4" r:id="rId3"/>
+    <sheet name="Three Puzzles" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="89">
   <si>
     <t>Solver Type</t>
   </si>
@@ -259,6 +260,30 @@
   </si>
   <si>
     <t>Input Puzzle #2</t>
+  </si>
+  <si>
+    <t>Pomeranz Puzzle ID</t>
+  </si>
+  <si>
+    <t># Best Buddies</t>
+  </si>
+  <si>
+    <t>Total Best Buddy Accuracy (%)</t>
+  </si>
+  <si>
+    <t>Best Buddy Density</t>
+  </si>
+  <si>
+    <t>Interior Best Buddy Accuracy (%)</t>
+  </si>
+  <si>
+    <t>Exterior Best Buddy Accuracy (%)</t>
+  </si>
+  <si>
+    <t>Number Wrong Interior Best Buddies</t>
+  </si>
+  <si>
+    <t>Number Wrong Exterior Best Buddies</t>
   </si>
 </sst>
 </file>
@@ -791,7 +816,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -816,6 +841,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1160,39 +1191,649 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C11:C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="14" style="8" customWidth="1"/>
+    <col min="5" max="6" width="18.7109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" style="8" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2024</v>
+      </c>
+      <c r="C2" s="3">
+        <v>96.15</v>
+      </c>
+      <c r="D2" s="3">
+        <v>62.86</v>
+      </c>
+      <c r="E2" s="3">
+        <v>96.62</v>
+      </c>
+      <c r="F2" s="12">
+        <f>100*(1-H2/81)</f>
+        <v>87.654320987654316</v>
+      </c>
+      <c r="G2" s="3">
+        <v>68</v>
+      </c>
+      <c r="H2" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2164</v>
+      </c>
+      <c r="C3" s="3">
+        <v>97.6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>67.2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>97.82</v>
+      </c>
+      <c r="F3" s="12">
+        <f t="shared" ref="F3:F21" si="0">100*(1-H3/81)</f>
+        <v>93.827160493827151</v>
+      </c>
+      <c r="G3" s="3">
+        <v>47</v>
+      </c>
+      <c r="H3" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <f t="shared" ref="A4:A21" si="1">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2148</v>
+      </c>
+      <c r="C4" s="4">
+        <v>94.32</v>
+      </c>
+      <c r="D4" s="4">
+        <v>66.709999999999994</v>
+      </c>
+      <c r="E4" s="4">
+        <v>94.94</v>
+      </c>
+      <c r="F4" s="13">
+        <f t="shared" si="0"/>
+        <v>82.716049382716051</v>
+      </c>
+      <c r="G4" s="4">
+        <v>108</v>
+      </c>
+      <c r="H4" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2052</v>
+      </c>
+      <c r="C5" s="3">
+        <v>94.64</v>
+      </c>
+      <c r="D5" s="3">
+        <v>63.73</v>
+      </c>
+      <c r="E5" s="3">
+        <v>94.92</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" si="0"/>
+        <v>92.592592592592595</v>
+      </c>
+      <c r="G5" s="3">
+        <v>104</v>
+      </c>
+      <c r="H5" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2410</v>
+      </c>
+      <c r="C6" s="3">
+        <v>98.51</v>
+      </c>
+      <c r="D6" s="3">
+        <v>74.84</v>
+      </c>
+      <c r="E6" s="3">
+        <v>98.88</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" si="0"/>
+        <v>88.888888888888886</v>
+      </c>
+      <c r="G6" s="3">
+        <v>27</v>
+      </c>
+      <c r="H6" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2362</v>
+      </c>
+      <c r="C7" s="3">
+        <v>98.14</v>
+      </c>
+      <c r="D7" s="3">
+        <v>73.349999999999994</v>
+      </c>
+      <c r="E7" s="3">
+        <v>98.35</v>
+      </c>
+      <c r="F7" s="12">
+        <f t="shared" si="0"/>
+        <v>93.827160493827151</v>
+      </c>
+      <c r="G7" s="3">
+        <v>39</v>
+      </c>
+      <c r="H7" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2514</v>
+      </c>
+      <c r="C8" s="3">
+        <v>99.44</v>
+      </c>
+      <c r="D8" s="3">
+        <v>78.069999999999993</v>
+      </c>
+      <c r="E8" s="3">
+        <v>99.52</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" si="0"/>
+        <v>97.53086419753086</v>
+      </c>
+      <c r="G8" s="3">
+        <v>12</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2292</v>
+      </c>
+      <c r="C9" s="3">
+        <v>98.5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>71.180000000000007</v>
+      </c>
+      <c r="E9" s="3">
+        <v>99.04</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" si="0"/>
+        <v>97.53086419753086</v>
+      </c>
+      <c r="G9" s="3">
+        <v>22</v>
+      </c>
+      <c r="H9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2152</v>
+      </c>
+      <c r="C10" s="3">
+        <v>97.3</v>
+      </c>
+      <c r="D10" s="3">
+        <v>66.83</v>
+      </c>
+      <c r="E10" s="3">
+        <v>97.71</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="0"/>
+        <v>88.888888888888886</v>
+      </c>
+      <c r="G10" s="3">
+        <v>49</v>
+      </c>
+      <c r="H10" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2522</v>
+      </c>
+      <c r="C11" s="3">
+        <v>99.29</v>
+      </c>
+      <c r="D11" s="3">
+        <v>78.319999999999993</v>
+      </c>
+      <c r="E11" s="3">
+        <v>99.44</v>
+      </c>
+      <c r="F11" s="12">
+        <f t="shared" si="0"/>
+        <v>95.061728395061735</v>
+      </c>
+      <c r="G11" s="3">
+        <v>14</v>
+      </c>
+      <c r="H11" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2566</v>
+      </c>
+      <c r="C12" s="3">
+        <v>98.99</v>
+      </c>
+      <c r="D12" s="3">
+        <v>79.69</v>
+      </c>
+      <c r="E12" s="3">
+        <v>99.1</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="0"/>
+        <v>96.296296296296305</v>
+      </c>
+      <c r="G12" s="3">
+        <v>23</v>
+      </c>
+      <c r="H12" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1780</v>
+      </c>
+      <c r="C13" s="4">
+        <v>97.19</v>
+      </c>
+      <c r="D13" s="4">
+        <v>55.28</v>
+      </c>
+      <c r="E13" s="4">
+        <v>97.68</v>
+      </c>
+      <c r="F13" s="13">
+        <f t="shared" si="0"/>
+        <v>88.888888888888886</v>
+      </c>
+      <c r="G13" s="4">
+        <v>41</v>
+      </c>
+      <c r="H13" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2510</v>
+      </c>
+      <c r="C14" s="3">
+        <v>99.6</v>
+      </c>
+      <c r="D14" s="3">
+        <v>77.95</v>
+      </c>
+      <c r="E14" s="3">
+        <v>99.8</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" si="0"/>
+        <v>93.827160493827151</v>
+      </c>
+      <c r="G14" s="3">
+        <v>5</v>
+      </c>
+      <c r="H14" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2746</v>
+      </c>
+      <c r="C15" s="3">
+        <v>99.85</v>
+      </c>
+      <c r="D15" s="3">
+        <v>85.28</v>
+      </c>
+      <c r="E15" s="3">
+        <v>99.93</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" si="0"/>
+        <v>97.53086419753086</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2462</v>
+      </c>
+      <c r="C16" s="3">
+        <v>98.78</v>
+      </c>
+      <c r="D16" s="3">
+        <v>76.45</v>
+      </c>
+      <c r="E16" s="3">
+        <v>99.06</v>
+      </c>
+      <c r="F16" s="12">
+        <f t="shared" si="0"/>
+        <v>91.358024691358025</v>
+      </c>
+      <c r="G16" s="3">
+        <v>23</v>
+      </c>
+      <c r="H16" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="4">
+        <v>2074</v>
+      </c>
+      <c r="C17" s="4">
+        <v>94.7</v>
+      </c>
+      <c r="D17" s="4">
+        <v>64.41</v>
+      </c>
+      <c r="E17" s="4">
+        <v>95.53</v>
+      </c>
+      <c r="F17" s="13">
+        <f t="shared" si="0"/>
+        <v>77.777777777777786</v>
+      </c>
+      <c r="G17" s="4">
+        <v>92</v>
+      </c>
+      <c r="H17" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="3">
+        <v>2374</v>
+      </c>
+      <c r="C18" s="3">
+        <v>98.65</v>
+      </c>
+      <c r="D18" s="3">
+        <v>73.73</v>
+      </c>
+      <c r="E18" s="3">
+        <v>99.03</v>
+      </c>
+      <c r="F18" s="12">
+        <f t="shared" si="0"/>
+        <v>88.888888888888886</v>
+      </c>
+      <c r="G18" s="3">
+        <v>23</v>
+      </c>
+      <c r="H18" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="3">
+        <v>2142</v>
+      </c>
+      <c r="C19" s="3">
+        <v>98.13</v>
+      </c>
+      <c r="D19" s="3">
+        <v>66.52</v>
+      </c>
+      <c r="E19" s="3">
+        <v>98.73</v>
+      </c>
+      <c r="F19" s="12">
+        <f t="shared" si="0"/>
+        <v>83.950617283950606</v>
+      </c>
+      <c r="G19" s="3">
+        <v>27</v>
+      </c>
+      <c r="H19" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="3">
+        <v>2532</v>
+      </c>
+      <c r="C20" s="3">
+        <v>99.05</v>
+      </c>
+      <c r="D20" s="3">
+        <v>78.63</v>
+      </c>
+      <c r="E20" s="3">
+        <v>99.41</v>
+      </c>
+      <c r="F20" s="12">
+        <f t="shared" si="0"/>
+        <v>88.888888888888886</v>
+      </c>
+      <c r="G20" s="3">
+        <v>15</v>
+      </c>
+      <c r="H20" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="3">
+        <v>2700</v>
+      </c>
+      <c r="C21" s="3">
+        <v>98.91</v>
+      </c>
+      <c r="D21" s="3">
+        <v>83.85</v>
+      </c>
+      <c r="E21" s="3">
+        <v>99.37</v>
+      </c>
+      <c r="F21" s="12">
+        <f t="shared" si="0"/>
+        <v>81.481481481481495</v>
+      </c>
+      <c r="G21" s="3">
+        <v>17</v>
+      </c>
+      <c r="H21" s="3">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="7" customWidth="1"/>
     <col min="2" max="2" width="9" style="7"/>
-    <col min="3" max="3" width="29.125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="12.875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.25" style="7" customWidth="1"/>
-    <col min="6" max="6" width="21.875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="21.875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="14.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="15.25" style="7" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="9.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="13" width="12.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="11.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="12.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="15.25" style="7" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.125" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="9.375" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="20" width="12.375" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="11.375" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="12.375" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="15.625" style="7" customWidth="1"/>
-    <col min="24" max="24" width="12.25" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="17.375" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.75" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="15.875" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="29.140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="14.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="15.28515625" style="7" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.140625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="9.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="13" width="12.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="11.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="12.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="15.28515625" style="7" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.140625" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="9.42578125" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="20" width="12.42578125" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="11.42578125" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="12.42578125" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="15.5703125" style="7" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="17.42578125" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.7109375" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="15.85546875" style="7" customWidth="1" outlineLevel="1"/>
     <col min="28" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
@@ -4683,7 +5324,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW49"/>
   <sheetViews>
@@ -4691,52 +5332,52 @@
       <selection activeCell="AR48" sqref="A48:AR48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="7" customWidth="1"/>
     <col min="2" max="2" width="9" style="7"/>
-    <col min="3" max="3" width="31.875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.25" style="7" customWidth="1"/>
-    <col min="6" max="6" width="21.875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="21.875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="14.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="15.25" style="7" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="9.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="13" width="12.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="11.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="12.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="15.25" style="7" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="9.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="20" width="12.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="11.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="12.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="15.625" style="7" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="12.25" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="17.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.75" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="15.875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="21.875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="15.25" style="8" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="34" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="35" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="37" max="37" width="15.25" style="8" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="39" max="39" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="41" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="42" max="42" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="43" max="43" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="44" max="44" width="15.625" style="8" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="46" max="46" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="48" max="48" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="31.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="14.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="15.28515625" style="7" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.140625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="9.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="13" width="12.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="11.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="12.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="15.28515625" style="7" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.140625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="9.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="20" width="12.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="11.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="12.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="15.5703125" style="7" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.28515625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="17.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.7109375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="15.85546875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="21.85546875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="15.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="34" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="37" max="37" width="15.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="39" max="39" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="41" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="42" max="42" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="43" max="43" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="44" max="44" width="15.5703125" style="8" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="46" max="46" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="48" max="48" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="49" max="49" width="9" style="8" collapsed="1"/>
     <col min="50" max="16384" width="9" style="8"/>
   </cols>
@@ -11870,7 +12511,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR4"/>
   <sheetViews>
@@ -11878,71 +12519,71 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="8" customWidth="1"/>
     <col min="2" max="2" width="9" style="8"/>
-    <col min="3" max="3" width="46.25" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12.875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="13.25" style="8" customWidth="1"/>
-    <col min="6" max="6" width="21.875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="15.25" style="8" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="13" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="15.25" style="8" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="9.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="20" width="12.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="11.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="12.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="15.625" style="8" customWidth="1"/>
-    <col min="24" max="24" width="12.25" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="17.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.75" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="15.875" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="21.875" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="14.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="15.25" style="8" customWidth="1"/>
-    <col min="31" max="31" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="34" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="35" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="37" max="37" width="15.25" style="8" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="39" max="39" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="41" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="42" max="42" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="43" max="43" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="44" max="44" width="15.625" style="8" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="46" max="46" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="48" max="48" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="49" max="49" width="15.625" style="8" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="12.25" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="51" max="51" width="17.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.75" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="53" max="53" width="15.875" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="54" max="54" width="21.875" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="55" max="55" width="14.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="56" max="56" width="15.25" style="8" customWidth="1"/>
-    <col min="57" max="57" width="14.125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="58" max="58" width="9.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="60" width="12.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="61" max="61" width="11.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="62" max="62" width="12.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="63" max="63" width="15.25" style="8" customWidth="1"/>
-    <col min="64" max="64" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="65" max="65" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="67" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="69" max="69" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="46.28515625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="15.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="13" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="15.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.140625" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="9.42578125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="20" width="12.42578125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="11.42578125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="12.42578125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="15.5703125" style="8" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="17.42578125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.7109375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="15.85546875" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="21.85546875" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="14.42578125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="15.28515625" style="8" customWidth="1"/>
+    <col min="31" max="31" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="34" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="37" max="37" width="15.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="39" max="39" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="41" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="42" max="42" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="43" max="43" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="44" max="44" width="15.5703125" style="8" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="46" max="46" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="48" max="48" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="49" max="49" width="15.5703125" style="8" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="12.28515625" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="51" max="51" width="17.42578125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.7109375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="53" max="53" width="15.85546875" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="54" max="54" width="21.85546875" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="55" max="55" width="14.42578125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="56" max="56" width="15.28515625" style="8" customWidth="1"/>
+    <col min="57" max="57" width="14.140625" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="58" max="58" width="9.42578125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="60" width="12.42578125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="61" max="61" width="11.42578125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="12.42578125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="63" max="63" width="15.28515625" style="8" customWidth="1"/>
+    <col min="64" max="64" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="65" max="65" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="67" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="69" max="69" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="70" max="70" width="9" style="8" collapsed="1"/>
     <col min="71" max="16384" width="9" style="8"/>
   </cols>

</xml_diff>

<commit_message>
Uploading more best buddy analysis data.
</commit_message>
<xml_diff>
--- a/Reports/Thesis/results/Pomeranz 805 Piece Puzzle Results.xlsx
+++ b/Reports/Thesis/results/Pomeranz 805 Piece Puzzle Results.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27960" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27960" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
-    <sheet name="One Puzzle" sheetId="3" r:id="rId2"/>
-    <sheet name="Two Puzzles" sheetId="4" r:id="rId3"/>
-    <sheet name="Three Puzzles" sheetId="5" r:id="rId4"/>
+    <sheet name="Cho Best Buddies" sheetId="7" r:id="rId1"/>
+    <sheet name="Mcgill Best Buddies" sheetId="9" r:id="rId2"/>
+    <sheet name="Pomeranz Best Buddies" sheetId="6" r:id="rId3"/>
+    <sheet name="One Puzzle" sheetId="3" r:id="rId4"/>
+    <sheet name="Two Puzzles" sheetId="4" r:id="rId5"/>
+    <sheet name="Three Puzzles" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="90">
   <si>
     <t>Solver Type</t>
   </si>
@@ -284,6 +286,9 @@
   </si>
   <si>
     <t>Number Wrong Exterior Best Buddies</t>
+  </si>
+  <si>
+    <t>Cho Puzzle ID</t>
   </si>
 </sst>
 </file>
@@ -816,7 +821,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -834,6 +839,12 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -843,10 +854,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1193,25 +1201,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C11:C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="14" style="8" customWidth="1"/>
-    <col min="5" max="6" width="18.7109375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" style="8" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="11.375" customWidth="1"/>
+    <col min="2" max="2" width="10.375" customWidth="1"/>
+    <col min="3" max="3" width="13.75" customWidth="1"/>
+    <col min="4" max="4" width="12.625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="17.25" customWidth="1"/>
+    <col min="7" max="7" width="18.125" customWidth="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>82</v>
@@ -1240,558 +1248,558 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>2024</v>
+        <v>924</v>
       </c>
       <c r="C2" s="3">
-        <v>96.15</v>
+        <v>96.75</v>
       </c>
       <c r="D2" s="3">
-        <v>62.86</v>
+        <v>53.47</v>
       </c>
       <c r="E2" s="3">
-        <v>96.62</v>
-      </c>
-      <c r="F2" s="12">
-        <f>100*(1-H2/81)</f>
-        <v>87.654320987654316</v>
+        <v>97.49</v>
+      </c>
+      <c r="F2" s="9">
+        <f>100*(1-H2/84)</f>
+        <v>91.666666666666657</v>
       </c>
       <c r="G2" s="3">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="H2" s="3">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="5">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="3">
-        <v>2164</v>
-      </c>
-      <c r="C3" s="3">
-        <v>97.6</v>
-      </c>
-      <c r="D3" s="3">
-        <v>67.2</v>
-      </c>
-      <c r="E3" s="3">
-        <v>97.82</v>
-      </c>
-      <c r="F3" s="12">
-        <f t="shared" ref="F3:F21" si="0">100*(1-H3/81)</f>
-        <v>93.827160493827151</v>
-      </c>
-      <c r="G3" s="3">
-        <v>47</v>
-      </c>
-      <c r="H3" s="3">
+      <c r="B3" s="5">
+        <v>1124</v>
+      </c>
+      <c r="C3" s="5">
+        <v>97.15</v>
+      </c>
+      <c r="D3" s="5">
+        <v>65.05</v>
+      </c>
+      <c r="E3" s="5">
+        <v>97.59</v>
+      </c>
+      <c r="F3" s="14">
+        <f t="shared" ref="F3:F21" si="0">100*(1-H3/84)</f>
+        <v>94.047619047619051</v>
+      </c>
+      <c r="G3" s="5">
+        <v>27</v>
+      </c>
+      <c r="H3" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="5">
         <f t="shared" ref="A4:A21" si="1">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="4">
-        <v>2148</v>
-      </c>
-      <c r="C4" s="4">
-        <v>94.32</v>
-      </c>
-      <c r="D4" s="4">
-        <v>66.709999999999994</v>
-      </c>
-      <c r="E4" s="4">
-        <v>94.94</v>
-      </c>
-      <c r="F4" s="13">
+      <c r="B4" s="5">
+        <v>1356</v>
+      </c>
+      <c r="C4" s="5">
+        <v>98.82</v>
+      </c>
+      <c r="D4" s="5">
+        <v>78.47</v>
+      </c>
+      <c r="E4" s="5">
+        <v>99.04</v>
+      </c>
+      <c r="F4" s="14">
         <f t="shared" si="0"/>
-        <v>82.716049382716051</v>
-      </c>
-      <c r="G4" s="4">
-        <v>108</v>
-      </c>
-      <c r="H4" s="4">
-        <v>14</v>
+        <v>96.428571428571431</v>
+      </c>
+      <c r="G4" s="5">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="5">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>2052</v>
-      </c>
-      <c r="C5" s="3">
-        <v>94.64</v>
-      </c>
-      <c r="D5" s="3">
-        <v>63.73</v>
-      </c>
-      <c r="E5" s="3">
-        <v>94.92</v>
-      </c>
-      <c r="F5" s="12">
+      <c r="B5" s="5">
+        <v>858</v>
+      </c>
+      <c r="C5" s="5">
+        <v>99.07</v>
+      </c>
+      <c r="D5" s="5">
+        <v>49.65</v>
+      </c>
+      <c r="E5" s="5">
+        <v>99.77</v>
+      </c>
+      <c r="F5" s="14">
         <f t="shared" si="0"/>
-        <v>92.592592592592595</v>
-      </c>
-      <c r="G5" s="3">
-        <v>104</v>
-      </c>
-      <c r="H5" s="3">
+        <v>92.857142857142861</v>
+      </c>
+      <c r="G5" s="5">
+        <v>2</v>
+      </c>
+      <c r="H5" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="5">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B6" s="3">
-        <v>2410</v>
-      </c>
-      <c r="C6" s="3">
-        <v>98.51</v>
-      </c>
-      <c r="D6" s="3">
-        <v>74.84</v>
-      </c>
-      <c r="E6" s="3">
-        <v>98.88</v>
-      </c>
-      <c r="F6" s="12">
+      <c r="B6" s="5">
+        <v>1364</v>
+      </c>
+      <c r="C6" s="5">
+        <v>98.68</v>
+      </c>
+      <c r="D6" s="5">
+        <v>78.94</v>
+      </c>
+      <c r="E6" s="5">
+        <v>99.41</v>
+      </c>
+      <c r="F6" s="14">
         <f t="shared" si="0"/>
-        <v>88.888888888888886</v>
-      </c>
-      <c r="G6" s="3">
-        <v>27</v>
-      </c>
-      <c r="H6" s="3">
-        <v>9</v>
+        <v>88.095238095238088</v>
+      </c>
+      <c r="G6" s="5">
+        <v>8</v>
+      </c>
+      <c r="H6" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="5">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B7" s="3">
-        <v>2362</v>
-      </c>
-      <c r="C7" s="3">
-        <v>98.14</v>
-      </c>
-      <c r="D7" s="3">
-        <v>73.349999999999994</v>
-      </c>
-      <c r="E7" s="3">
-        <v>98.35</v>
-      </c>
-      <c r="F7" s="12">
+      <c r="B7" s="5">
+        <v>1118</v>
+      </c>
+      <c r="C7" s="5">
+        <v>96.42</v>
+      </c>
+      <c r="D7" s="5">
+        <v>64.7</v>
+      </c>
+      <c r="E7" s="5">
+        <v>96.86</v>
+      </c>
+      <c r="F7" s="14">
         <f t="shared" si="0"/>
-        <v>93.827160493827151</v>
-      </c>
-      <c r="G7" s="3">
-        <v>39</v>
-      </c>
-      <c r="H7" s="3">
+        <v>94.047619047619051</v>
+      </c>
+      <c r="G7" s="5">
+        <v>35</v>
+      </c>
+      <c r="H7" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="5">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B8" s="3">
-        <v>2514</v>
-      </c>
-      <c r="C8" s="3">
-        <v>99.44</v>
-      </c>
-      <c r="D8" s="3">
-        <v>78.069999999999993</v>
-      </c>
-      <c r="E8" s="3">
-        <v>99.52</v>
-      </c>
-      <c r="F8" s="12">
+      <c r="B8" s="5">
+        <v>1136</v>
+      </c>
+      <c r="C8" s="5">
+        <v>98.59</v>
+      </c>
+      <c r="D8" s="5">
+        <v>65.739999999999995</v>
+      </c>
+      <c r="E8" s="5">
+        <v>98.59</v>
+      </c>
+      <c r="F8" s="14">
         <f t="shared" si="0"/>
-        <v>97.53086419753086</v>
-      </c>
-      <c r="G8" s="3">
-        <v>12</v>
-      </c>
-      <c r="H8" s="3">
-        <v>2</v>
+        <v>100</v>
+      </c>
+      <c r="G8" s="5">
+        <v>16</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="5">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B9" s="3">
-        <v>2292</v>
-      </c>
-      <c r="C9" s="3">
-        <v>98.5</v>
-      </c>
-      <c r="D9" s="3">
-        <v>71.180000000000007</v>
-      </c>
-      <c r="E9" s="3">
-        <v>99.04</v>
-      </c>
-      <c r="F9" s="12">
+      <c r="B9" s="5">
+        <v>1522</v>
+      </c>
+      <c r="C9" s="5">
+        <v>99.34</v>
+      </c>
+      <c r="D9" s="5">
+        <v>88.08</v>
+      </c>
+      <c r="E9" s="5">
+        <v>99.87</v>
+      </c>
+      <c r="F9" s="14">
         <f t="shared" si="0"/>
-        <v>97.53086419753086</v>
-      </c>
-      <c r="G9" s="3">
-        <v>22</v>
-      </c>
-      <c r="H9" s="3">
-        <v>2</v>
+        <v>90.476190476190482</v>
+      </c>
+      <c r="G9" s="5">
+        <v>2</v>
+      </c>
+      <c r="H9" s="5">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="5">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B10" s="3">
-        <v>2152</v>
-      </c>
-      <c r="C10" s="3">
-        <v>97.3</v>
-      </c>
-      <c r="D10" s="3">
-        <v>66.83</v>
-      </c>
-      <c r="E10" s="3">
-        <v>97.71</v>
-      </c>
-      <c r="F10" s="12">
+      <c r="B10" s="5">
+        <v>1270</v>
+      </c>
+      <c r="C10" s="5">
+        <v>97.64</v>
+      </c>
+      <c r="D10" s="5">
+        <v>73.5</v>
+      </c>
+      <c r="E10" s="5">
+        <v>98.57</v>
+      </c>
+      <c r="F10" s="14">
         <f t="shared" si="0"/>
-        <v>88.888888888888886</v>
-      </c>
-      <c r="G10" s="3">
-        <v>49</v>
-      </c>
-      <c r="H10" s="3">
-        <v>9</v>
+        <v>85.714285714285722</v>
+      </c>
+      <c r="G10" s="5">
+        <v>18</v>
+      </c>
+      <c r="H10" s="5">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" s="3">
-        <v>2522</v>
+        <v>1288</v>
       </c>
       <c r="C11" s="3">
-        <v>99.29</v>
+        <v>99.07</v>
       </c>
       <c r="D11" s="3">
-        <v>78.319999999999993</v>
+        <v>74.540000000000006</v>
       </c>
       <c r="E11" s="3">
-        <v>99.44</v>
-      </c>
-      <c r="F11" s="12">
-        <f t="shared" si="0"/>
-        <v>95.061728395061735</v>
+        <v>99.15</v>
+      </c>
+      <c r="F11" s="9">
+        <f>100*(1-H11/84)</f>
+        <v>98.80952380952381</v>
       </c>
       <c r="G11" s="3">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H11" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="5">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B12" s="3">
-        <v>2566</v>
-      </c>
-      <c r="C12" s="3">
-        <v>98.99</v>
-      </c>
-      <c r="D12" s="3">
-        <v>79.69</v>
-      </c>
-      <c r="E12" s="3">
-        <v>99.1</v>
-      </c>
-      <c r="F12" s="12">
+      <c r="B12" s="5">
+        <v>1324</v>
+      </c>
+      <c r="C12" s="5">
+        <v>98.94</v>
+      </c>
+      <c r="D12" s="5">
+        <v>76.62</v>
+      </c>
+      <c r="E12" s="5">
+        <v>99.24</v>
+      </c>
+      <c r="F12" s="14">
         <f t="shared" si="0"/>
-        <v>96.296296296296305</v>
-      </c>
-      <c r="G12" s="3">
-        <v>23</v>
-      </c>
-      <c r="H12" s="3">
-        <v>3</v>
+        <v>95.238095238095227</v>
+      </c>
+      <c r="G12" s="5">
+        <v>10</v>
+      </c>
+      <c r="H12" s="5">
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B13" s="4">
-        <v>1780</v>
-      </c>
-      <c r="C13" s="4">
-        <v>97.19</v>
-      </c>
-      <c r="D13" s="4">
-        <v>55.28</v>
-      </c>
-      <c r="E13" s="4">
-        <v>97.68</v>
-      </c>
-      <c r="F13" s="13">
+      <c r="B13" s="5">
+        <v>1424</v>
+      </c>
+      <c r="C13" s="5">
+        <v>96.77</v>
+      </c>
+      <c r="D13" s="5">
+        <v>82.41</v>
+      </c>
+      <c r="E13" s="5">
+        <v>97.39</v>
+      </c>
+      <c r="F13" s="14">
         <f t="shared" si="0"/>
-        <v>88.888888888888886</v>
-      </c>
-      <c r="G13" s="4">
-        <v>41</v>
-      </c>
-      <c r="H13" s="4">
+        <v>89.285714285714292</v>
+      </c>
+      <c r="G13" s="5">
+        <v>37</v>
+      </c>
+      <c r="H13" s="5">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="5">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B14" s="3">
-        <v>2510</v>
-      </c>
-      <c r="C14" s="3">
-        <v>99.6</v>
-      </c>
-      <c r="D14" s="3">
-        <v>77.95</v>
-      </c>
-      <c r="E14" s="3">
-        <v>99.8</v>
-      </c>
-      <c r="F14" s="12">
-        <f t="shared" si="0"/>
-        <v>93.827160493827151</v>
-      </c>
-      <c r="G14" s="3">
-        <v>5</v>
-      </c>
-      <c r="H14" s="3">
-        <v>5</v>
+      <c r="B14" s="5">
+        <v>1124</v>
+      </c>
+      <c r="C14" s="5">
+        <v>99.29</v>
+      </c>
+      <c r="D14" s="5">
+        <v>65.05</v>
+      </c>
+      <c r="E14" s="5">
+        <v>99.29</v>
+      </c>
+      <c r="F14" s="14">
+        <f>100*(1-H14/84)</f>
+        <v>100</v>
+      </c>
+      <c r="G14" s="5">
+        <v>8</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B15" s="3">
-        <v>2746</v>
-      </c>
-      <c r="C15" s="3">
-        <v>99.85</v>
-      </c>
-      <c r="D15" s="3">
-        <v>85.28</v>
-      </c>
-      <c r="E15" s="3">
-        <v>99.93</v>
-      </c>
-      <c r="F15" s="12">
+      <c r="B15" s="5">
+        <v>1504</v>
+      </c>
+      <c r="C15" s="5">
+        <v>99.07</v>
+      </c>
+      <c r="D15" s="5">
+        <v>87.04</v>
+      </c>
+      <c r="E15" s="5">
+        <v>99.6</v>
+      </c>
+      <c r="F15" s="14">
         <f t="shared" si="0"/>
-        <v>97.53086419753086</v>
-      </c>
-      <c r="G15" s="3">
-        <v>2</v>
-      </c>
-      <c r="H15" s="3">
-        <v>2</v>
+        <v>90.476190476190482</v>
+      </c>
+      <c r="G15" s="5">
+        <v>6</v>
+      </c>
+      <c r="H15" s="5">
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B16" s="3">
-        <v>2462</v>
-      </c>
-      <c r="C16" s="3">
-        <v>98.78</v>
-      </c>
-      <c r="D16" s="3">
-        <v>76.45</v>
-      </c>
-      <c r="E16" s="3">
-        <v>99.06</v>
-      </c>
-      <c r="F16" s="12">
+      <c r="B16" s="5">
+        <v>1124</v>
+      </c>
+      <c r="C16" s="5">
+        <v>97.86</v>
+      </c>
+      <c r="D16" s="5">
+        <v>65.05</v>
+      </c>
+      <c r="E16" s="5">
+        <v>98.57</v>
+      </c>
+      <c r="F16" s="14">
         <f t="shared" si="0"/>
-        <v>91.358024691358025</v>
-      </c>
-      <c r="G16" s="3">
-        <v>23</v>
-      </c>
-      <c r="H16" s="3">
-        <v>7</v>
+        <v>90.476190476190482</v>
+      </c>
+      <c r="G16" s="5">
+        <v>16</v>
+      </c>
+      <c r="H16" s="5">
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="5">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B17" s="4">
-        <v>2074</v>
-      </c>
-      <c r="C17" s="4">
-        <v>94.7</v>
-      </c>
-      <c r="D17" s="4">
-        <v>64.41</v>
-      </c>
-      <c r="E17" s="4">
-        <v>95.53</v>
-      </c>
-      <c r="F17" s="13">
+      <c r="B17" s="5">
+        <v>1304</v>
+      </c>
+      <c r="C17" s="5">
+        <v>99.08</v>
+      </c>
+      <c r="D17" s="5">
+        <v>75.459999999999994</v>
+      </c>
+      <c r="E17" s="5">
+        <v>99.38</v>
+      </c>
+      <c r="F17" s="14">
         <f t="shared" si="0"/>
-        <v>77.777777777777786</v>
-      </c>
-      <c r="G17" s="4">
-        <v>92</v>
-      </c>
-      <c r="H17" s="4">
-        <v>18</v>
+        <v>95.238095238095227</v>
+      </c>
+      <c r="G17" s="5">
+        <v>8</v>
+      </c>
+      <c r="H17" s="5">
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="5">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B18" s="3">
-        <v>2374</v>
-      </c>
-      <c r="C18" s="3">
-        <v>98.65</v>
-      </c>
-      <c r="D18" s="3">
-        <v>73.73</v>
-      </c>
-      <c r="E18" s="3">
-        <v>99.03</v>
-      </c>
-      <c r="F18" s="12">
+      <c r="B18" s="5">
+        <v>1364</v>
+      </c>
+      <c r="C18" s="5">
+        <v>98.83</v>
+      </c>
+      <c r="D18" s="5">
+        <v>78.94</v>
+      </c>
+      <c r="E18" s="5">
+        <v>99.26</v>
+      </c>
+      <c r="F18" s="14">
         <f t="shared" si="0"/>
-        <v>88.888888888888886</v>
-      </c>
-      <c r="G18" s="3">
-        <v>23</v>
-      </c>
-      <c r="H18" s="3">
-        <v>9</v>
+        <v>92.857142857142861</v>
+      </c>
+      <c r="G18" s="5">
+        <v>10</v>
+      </c>
+      <c r="H18" s="5">
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="5">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B19" s="3">
-        <v>2142</v>
-      </c>
-      <c r="C19" s="3">
-        <v>98.13</v>
-      </c>
-      <c r="D19" s="3">
-        <v>66.52</v>
-      </c>
-      <c r="E19" s="3">
-        <v>98.73</v>
-      </c>
-      <c r="F19" s="12">
+      <c r="B19" s="5">
+        <v>1288</v>
+      </c>
+      <c r="C19" s="5">
+        <v>98.45</v>
+      </c>
+      <c r="D19" s="5">
+        <v>74.540000000000006</v>
+      </c>
+      <c r="E19" s="5">
+        <v>98.99</v>
+      </c>
+      <c r="F19" s="14">
         <f t="shared" si="0"/>
-        <v>83.950617283950606</v>
-      </c>
-      <c r="G19" s="3">
-        <v>27</v>
-      </c>
-      <c r="H19" s="3">
+        <v>91.666666666666657</v>
+      </c>
+      <c r="G19" s="5">
         <v>13</v>
       </c>
+      <c r="H19" s="5">
+        <v>7</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="5">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B20" s="3">
-        <v>2532</v>
-      </c>
-      <c r="C20" s="3">
-        <v>99.05</v>
-      </c>
-      <c r="D20" s="3">
-        <v>78.63</v>
-      </c>
-      <c r="E20" s="3">
-        <v>99.41</v>
-      </c>
-      <c r="F20" s="12">
+      <c r="B20" s="5">
+        <v>1536</v>
+      </c>
+      <c r="C20" s="5">
+        <v>99.48</v>
+      </c>
+      <c r="D20" s="5">
+        <v>88.89</v>
+      </c>
+      <c r="E20" s="5">
+        <v>99.8</v>
+      </c>
+      <c r="F20" s="14">
         <f t="shared" si="0"/>
-        <v>88.888888888888886</v>
-      </c>
-      <c r="G20" s="3">
-        <v>15</v>
-      </c>
-      <c r="H20" s="3">
-        <v>9</v>
+        <v>94.047619047619051</v>
+      </c>
+      <c r="G20" s="5">
+        <v>3</v>
+      </c>
+      <c r="H20" s="5">
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="5">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B21" s="3">
-        <v>2700</v>
-      </c>
-      <c r="C21" s="3">
-        <v>98.91</v>
-      </c>
-      <c r="D21" s="3">
-        <v>83.85</v>
-      </c>
-      <c r="E21" s="3">
-        <v>99.37</v>
-      </c>
-      <c r="F21" s="12">
+      <c r="B21" s="5">
+        <v>1462</v>
+      </c>
+      <c r="C21" s="5">
+        <v>99.18</v>
+      </c>
+      <c r="D21" s="5">
+        <v>84.61</v>
+      </c>
+      <c r="E21" s="5">
+        <v>99.93</v>
+      </c>
+      <c r="F21" s="14">
         <f t="shared" si="0"/>
-        <v>81.481481481481495</v>
-      </c>
-      <c r="G21" s="3">
-        <v>17</v>
-      </c>
-      <c r="H21" s="3">
-        <v>15</v>
+        <v>86.904761904761912</v>
+      </c>
+      <c r="G21" s="5">
+        <v>1</v>
+      </c>
+      <c r="H21" s="5">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1800,6 +1808,1101 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="13.75" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="16" style="8" customWidth="1"/>
+    <col min="6" max="6" width="17.25" style="8" customWidth="1"/>
+    <col min="7" max="7" width="18.125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="17.5" style="8" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="9">
+        <f>100*(1-H2/94)</f>
+        <v>100</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="9">
+        <f t="shared" ref="F3:F21" si="0">100*(1-H3/94)</f>
+        <v>100</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <f t="shared" ref="A4:A21" si="1">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="9">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="9">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="9">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="9">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="10">
+        <f t="shared" si="0"/>
+        <v>94.680851063829792</v>
+      </c>
+      <c r="G8" s="4">
+        <v>3</v>
+      </c>
+      <c r="H8" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1134</v>
+      </c>
+      <c r="C9" s="5">
+        <v>93.83</v>
+      </c>
+      <c r="D9" s="5">
+        <v>52.5</v>
+      </c>
+      <c r="E9" s="5">
+        <v>94.49</v>
+      </c>
+      <c r="F9" s="9">
+        <f t="shared" si="0"/>
+        <v>91.489361702127653</v>
+      </c>
+      <c r="G9" s="5">
+        <v>62</v>
+      </c>
+      <c r="H9" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1356</v>
+      </c>
+      <c r="C10" s="5">
+        <v>95.72</v>
+      </c>
+      <c r="D10" s="5">
+        <v>62.78</v>
+      </c>
+      <c r="E10" s="5">
+        <v>95.79</v>
+      </c>
+      <c r="F10" s="9">
+        <f t="shared" si="0"/>
+        <v>98.936170212765958</v>
+      </c>
+      <c r="G10" s="5">
+        <v>57</v>
+      </c>
+      <c r="H10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="9">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="9">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="9">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="9">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1826</v>
+      </c>
+      <c r="C15" s="4">
+        <v>99.01</v>
+      </c>
+      <c r="D15" s="4">
+        <v>84.54</v>
+      </c>
+      <c r="E15" s="4">
+        <v>99.56</v>
+      </c>
+      <c r="F15" s="10">
+        <f t="shared" si="0"/>
+        <v>89.361702127659569</v>
+      </c>
+      <c r="G15" s="4">
+        <v>8</v>
+      </c>
+      <c r="H15" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1978</v>
+      </c>
+      <c r="C16" s="4">
+        <v>99.09</v>
+      </c>
+      <c r="D16" s="4">
+        <v>91.57</v>
+      </c>
+      <c r="E16" s="4">
+        <v>99.59</v>
+      </c>
+      <c r="F16" s="10">
+        <f t="shared" si="0"/>
+        <v>89.361702127659569</v>
+      </c>
+      <c r="G16" s="4">
+        <v>8</v>
+      </c>
+      <c r="H16" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1912</v>
+      </c>
+      <c r="C17" s="5">
+        <v>99.37</v>
+      </c>
+      <c r="D17" s="5">
+        <v>88.52</v>
+      </c>
+      <c r="E17" s="5">
+        <v>99.63</v>
+      </c>
+      <c r="F17" s="9">
+        <f t="shared" si="0"/>
+        <v>94.680851063829792</v>
+      </c>
+      <c r="G17" s="5">
+        <v>7</v>
+      </c>
+      <c r="H17" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1242</v>
+      </c>
+      <c r="C18" s="5">
+        <v>95.97</v>
+      </c>
+      <c r="D18" s="5">
+        <v>57.5</v>
+      </c>
+      <c r="E18" s="5">
+        <v>96.52</v>
+      </c>
+      <c r="F18" s="9">
+        <f t="shared" si="0"/>
+        <v>92.553191489361694</v>
+      </c>
+      <c r="G18" s="5">
+        <v>43</v>
+      </c>
+      <c r="H18" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1314</v>
+      </c>
+      <c r="C19" s="5">
+        <v>98.17</v>
+      </c>
+      <c r="D19" s="5">
+        <v>60.83</v>
+      </c>
+      <c r="E19" s="5">
+        <v>98.25</v>
+      </c>
+      <c r="F19" s="9">
+        <f t="shared" si="0"/>
+        <v>98.936170212765958</v>
+      </c>
+      <c r="G19" s="5">
+        <v>23</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1644</v>
+      </c>
+      <c r="C20" s="5">
+        <v>98.54</v>
+      </c>
+      <c r="D20" s="5">
+        <v>76.11</v>
+      </c>
+      <c r="E20" s="5">
+        <v>98.9</v>
+      </c>
+      <c r="F20" s="9">
+        <f t="shared" si="0"/>
+        <v>93.61702127659575</v>
+      </c>
+      <c r="G20" s="5">
+        <v>18</v>
+      </c>
+      <c r="H20" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1662</v>
+      </c>
+      <c r="C21" s="5">
+        <v>97.59</v>
+      </c>
+      <c r="D21" s="5">
+        <v>76.94</v>
+      </c>
+      <c r="E21" s="5">
+        <v>98.07</v>
+      </c>
+      <c r="F21" s="9">
+        <f t="shared" si="0"/>
+        <v>91.489361702127653</v>
+      </c>
+      <c r="G21" s="5">
+        <v>32</v>
+      </c>
+      <c r="H21" s="5">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="13.875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="17.125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="14" style="8" customWidth="1"/>
+    <col min="5" max="6" width="18.75" style="8" customWidth="1"/>
+    <col min="7" max="7" width="20.625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="19.625" style="8" customWidth="1"/>
+    <col min="9" max="16384" width="9.125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2024</v>
+      </c>
+      <c r="C2" s="3">
+        <v>96.15</v>
+      </c>
+      <c r="D2" s="3">
+        <v>62.86</v>
+      </c>
+      <c r="E2" s="3">
+        <v>96.62</v>
+      </c>
+      <c r="F2" s="9">
+        <f>100*(1-H2/116)</f>
+        <v>91.379310344827587</v>
+      </c>
+      <c r="G2" s="3">
+        <v>68</v>
+      </c>
+      <c r="H2" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2164</v>
+      </c>
+      <c r="C3" s="3">
+        <v>97.6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>67.2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>97.82</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" ref="F3:F21" si="0">100*(1-H3/116)</f>
+        <v>95.689655172413794</v>
+      </c>
+      <c r="G3" s="3">
+        <v>47</v>
+      </c>
+      <c r="H3" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <f t="shared" ref="A4:A21" si="1">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2148</v>
+      </c>
+      <c r="C4" s="4">
+        <v>94.32</v>
+      </c>
+      <c r="D4" s="4">
+        <v>66.709999999999994</v>
+      </c>
+      <c r="E4" s="4">
+        <v>94.94</v>
+      </c>
+      <c r="F4" s="10">
+        <f t="shared" si="0"/>
+        <v>87.931034482758619</v>
+      </c>
+      <c r="G4" s="4">
+        <v>108</v>
+      </c>
+      <c r="H4" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2052</v>
+      </c>
+      <c r="C5" s="3">
+        <v>94.64</v>
+      </c>
+      <c r="D5" s="3">
+        <v>63.73</v>
+      </c>
+      <c r="E5" s="3">
+        <v>94.92</v>
+      </c>
+      <c r="F5" s="9">
+        <f t="shared" si="0"/>
+        <v>94.827586206896555</v>
+      </c>
+      <c r="G5" s="3">
+        <v>104</v>
+      </c>
+      <c r="H5" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2410</v>
+      </c>
+      <c r="C6" s="3">
+        <v>98.51</v>
+      </c>
+      <c r="D6" s="3">
+        <v>74.84</v>
+      </c>
+      <c r="E6" s="3">
+        <v>98.88</v>
+      </c>
+      <c r="F6" s="9">
+        <f t="shared" si="0"/>
+        <v>92.241379310344826</v>
+      </c>
+      <c r="G6" s="3">
+        <v>27</v>
+      </c>
+      <c r="H6" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2362</v>
+      </c>
+      <c r="C7" s="3">
+        <v>98.14</v>
+      </c>
+      <c r="D7" s="3">
+        <v>73.349999999999994</v>
+      </c>
+      <c r="E7" s="3">
+        <v>98.35</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" si="0"/>
+        <v>95.689655172413794</v>
+      </c>
+      <c r="G7" s="3">
+        <v>39</v>
+      </c>
+      <c r="H7" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2514</v>
+      </c>
+      <c r="C8" s="3">
+        <v>99.44</v>
+      </c>
+      <c r="D8" s="3">
+        <v>78.069999999999993</v>
+      </c>
+      <c r="E8" s="3">
+        <v>99.52</v>
+      </c>
+      <c r="F8" s="9">
+        <f t="shared" si="0"/>
+        <v>98.275862068965509</v>
+      </c>
+      <c r="G8" s="3">
+        <v>12</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2292</v>
+      </c>
+      <c r="C9" s="3">
+        <v>98.5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>71.180000000000007</v>
+      </c>
+      <c r="E9" s="3">
+        <v>99.04</v>
+      </c>
+      <c r="F9" s="9">
+        <f t="shared" si="0"/>
+        <v>98.275862068965509</v>
+      </c>
+      <c r="G9" s="3">
+        <v>22</v>
+      </c>
+      <c r="H9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2152</v>
+      </c>
+      <c r="C10" s="3">
+        <v>97.3</v>
+      </c>
+      <c r="D10" s="3">
+        <v>66.83</v>
+      </c>
+      <c r="E10" s="3">
+        <v>97.71</v>
+      </c>
+      <c r="F10" s="9">
+        <f t="shared" si="0"/>
+        <v>92.241379310344826</v>
+      </c>
+      <c r="G10" s="3">
+        <v>49</v>
+      </c>
+      <c r="H10" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2522</v>
+      </c>
+      <c r="C11" s="3">
+        <v>99.29</v>
+      </c>
+      <c r="D11" s="3">
+        <v>78.319999999999993</v>
+      </c>
+      <c r="E11" s="3">
+        <v>99.44</v>
+      </c>
+      <c r="F11" s="9">
+        <f t="shared" si="0"/>
+        <v>96.551724137931032</v>
+      </c>
+      <c r="G11" s="3">
+        <v>14</v>
+      </c>
+      <c r="H11" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2566</v>
+      </c>
+      <c r="C12" s="3">
+        <v>98.99</v>
+      </c>
+      <c r="D12" s="3">
+        <v>79.69</v>
+      </c>
+      <c r="E12" s="3">
+        <v>99.1</v>
+      </c>
+      <c r="F12" s="9">
+        <f t="shared" si="0"/>
+        <v>97.41379310344827</v>
+      </c>
+      <c r="G12" s="3">
+        <v>23</v>
+      </c>
+      <c r="H12" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1780</v>
+      </c>
+      <c r="C13" s="4">
+        <v>97.19</v>
+      </c>
+      <c r="D13" s="4">
+        <v>55.28</v>
+      </c>
+      <c r="E13" s="4">
+        <v>97.68</v>
+      </c>
+      <c r="F13" s="10">
+        <f t="shared" si="0"/>
+        <v>92.241379310344826</v>
+      </c>
+      <c r="G13" s="4">
+        <v>41</v>
+      </c>
+      <c r="H13" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2510</v>
+      </c>
+      <c r="C14" s="3">
+        <v>99.6</v>
+      </c>
+      <c r="D14" s="3">
+        <v>77.95</v>
+      </c>
+      <c r="E14" s="3">
+        <v>99.8</v>
+      </c>
+      <c r="F14" s="9">
+        <f t="shared" si="0"/>
+        <v>95.689655172413794</v>
+      </c>
+      <c r="G14" s="3">
+        <v>5</v>
+      </c>
+      <c r="H14" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2746</v>
+      </c>
+      <c r="C15" s="3">
+        <v>99.85</v>
+      </c>
+      <c r="D15" s="3">
+        <v>85.28</v>
+      </c>
+      <c r="E15" s="3">
+        <v>99.93</v>
+      </c>
+      <c r="F15" s="9">
+        <f t="shared" si="0"/>
+        <v>98.275862068965509</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2462</v>
+      </c>
+      <c r="C16" s="3">
+        <v>98.78</v>
+      </c>
+      <c r="D16" s="3">
+        <v>76.45</v>
+      </c>
+      <c r="E16" s="3">
+        <v>99.06</v>
+      </c>
+      <c r="F16" s="9">
+        <f t="shared" si="0"/>
+        <v>93.965517241379317</v>
+      </c>
+      <c r="G16" s="3">
+        <v>23</v>
+      </c>
+      <c r="H16" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="4">
+        <v>2074</v>
+      </c>
+      <c r="C17" s="4">
+        <v>94.7</v>
+      </c>
+      <c r="D17" s="4">
+        <v>64.41</v>
+      </c>
+      <c r="E17" s="4">
+        <v>95.53</v>
+      </c>
+      <c r="F17" s="10">
+        <f t="shared" si="0"/>
+        <v>84.482758620689651</v>
+      </c>
+      <c r="G17" s="4">
+        <v>92</v>
+      </c>
+      <c r="H17" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="3">
+        <v>2374</v>
+      </c>
+      <c r="C18" s="3">
+        <v>98.65</v>
+      </c>
+      <c r="D18" s="3">
+        <v>73.73</v>
+      </c>
+      <c r="E18" s="3">
+        <v>99.03</v>
+      </c>
+      <c r="F18" s="9">
+        <f t="shared" si="0"/>
+        <v>92.241379310344826</v>
+      </c>
+      <c r="G18" s="3">
+        <v>23</v>
+      </c>
+      <c r="H18" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="3">
+        <v>2142</v>
+      </c>
+      <c r="C19" s="3">
+        <v>98.13</v>
+      </c>
+      <c r="D19" s="3">
+        <v>66.52</v>
+      </c>
+      <c r="E19" s="3">
+        <v>98.73</v>
+      </c>
+      <c r="F19" s="9">
+        <f t="shared" si="0"/>
+        <v>88.793103448275872</v>
+      </c>
+      <c r="G19" s="3">
+        <v>27</v>
+      </c>
+      <c r="H19" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="3">
+        <v>2532</v>
+      </c>
+      <c r="C20" s="3">
+        <v>99.05</v>
+      </c>
+      <c r="D20" s="3">
+        <v>78.63</v>
+      </c>
+      <c r="E20" s="3">
+        <v>99.41</v>
+      </c>
+      <c r="F20" s="9">
+        <f t="shared" si="0"/>
+        <v>92.241379310344826</v>
+      </c>
+      <c r="G20" s="3">
+        <v>15</v>
+      </c>
+      <c r="H20" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="3">
+        <v>2700</v>
+      </c>
+      <c r="C21" s="3">
+        <v>98.91</v>
+      </c>
+      <c r="D21" s="3">
+        <v>83.85</v>
+      </c>
+      <c r="E21" s="3">
+        <v>99.37</v>
+      </c>
+      <c r="F21" s="9">
+        <f t="shared" si="0"/>
+        <v>87.068965517241381</v>
+      </c>
+      <c r="G21" s="3">
+        <v>17</v>
+      </c>
+      <c r="H21" s="3">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA42"/>
   <sheetViews>
@@ -1809,65 +2912,65 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="16.375" style="7" customWidth="1"/>
     <col min="2" max="2" width="9" style="7"/>
-    <col min="3" max="3" width="29.140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="14.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="15.28515625" style="7" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.140625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="9.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="13" width="12.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="11.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="12.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="15.28515625" style="7" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.140625" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="9.42578125" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="20" width="12.42578125" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="11.42578125" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="12.42578125" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="15.5703125" style="7" customWidth="1"/>
-    <col min="24" max="24" width="12.28515625" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="17.42578125" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.7109375" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="15.85546875" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="29.125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="12.875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.25" style="7" customWidth="1"/>
+    <col min="6" max="6" width="21.875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="21.875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="14.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="15.25" style="7" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="9.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="13" width="12.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="11.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="12.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="15.25" style="7" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.125" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="9.375" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="20" width="12.375" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="11.375" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="12.375" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="15.625" style="7" customWidth="1"/>
+    <col min="24" max="24" width="12.25" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="17.375" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.75" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="15.875" style="7" customWidth="1" outlineLevel="1"/>
     <col min="28" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="I1" s="10" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="I1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10" t="s">
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10" t="s">
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
     </row>
     <row r="2" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5324,7 +6427,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW49"/>
   <sheetViews>
@@ -5334,110 +6437,110 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="16.375" style="7" customWidth="1"/>
     <col min="2" max="2" width="9" style="7"/>
-    <col min="3" max="3" width="31.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="14.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="15.28515625" style="7" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.140625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="9.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="13" width="12.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="11.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="12.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="15.28515625" style="7" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.140625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="9.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="20" width="12.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="11.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="12.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="15.5703125" style="7" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="12.28515625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="17.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.7109375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="15.85546875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="21.85546875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="15.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="34" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="35" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="37" max="37" width="15.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="39" max="39" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="41" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="42" max="42" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="43" max="43" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="44" max="44" width="15.5703125" style="8" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="46" max="46" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="48" max="48" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="31.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.25" style="7" customWidth="1"/>
+    <col min="6" max="6" width="21.875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="21.875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="14.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="15.25" style="7" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="9.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="13" width="12.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="11.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="12.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="15.25" style="7" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="9.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="20" width="12.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="11.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="12.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="15.625" style="7" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.25" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="17.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.75" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="15.875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="21.875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="15.25" style="8" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="34" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="37" max="37" width="15.25" style="8" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="39" max="39" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="41" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="42" max="42" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="43" max="43" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="44" max="44" width="15.625" style="8" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="46" max="46" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="48" max="48" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="49" max="49" width="9" style="8" collapsed="1"/>
     <col min="50" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="I1" s="10" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="I1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10" t="s">
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10" t="s">
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AD1" s="10" t="s">
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AD1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10" t="s">
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10"/>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10"/>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="10" t="s">
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="11"/>
-      <c r="AT1" s="11"/>
-      <c r="AU1" s="11"/>
-      <c r="AV1" s="11"/>
+      <c r="AS1" s="13"/>
+      <c r="AT1" s="13"/>
+      <c r="AU1" s="13"/>
+      <c r="AV1" s="13"/>
     </row>
     <row r="2" spans="1:48" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -12511,7 +13614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR4"/>
   <sheetViews>
@@ -12521,154 +13624,154 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="16.375" style="8" customWidth="1"/>
     <col min="2" max="2" width="9" style="8"/>
-    <col min="3" max="3" width="46.28515625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="15.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="13" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="15.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.140625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="9.42578125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="20" width="12.42578125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="11.42578125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="12.42578125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="15.5703125" style="8" customWidth="1"/>
-    <col min="24" max="24" width="12.28515625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="17.42578125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.7109375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="15.85546875" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="21.85546875" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="14.42578125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="15.28515625" style="8" customWidth="1"/>
-    <col min="31" max="31" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="34" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="35" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="37" max="37" width="15.28515625" style="8" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="39" max="39" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="41" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="42" max="42" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="43" max="43" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="44" max="44" width="15.5703125" style="8" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="46" max="46" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="48" max="48" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="49" max="49" width="15.5703125" style="8" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="12.28515625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="51" max="51" width="17.42578125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.7109375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="53" max="53" width="15.85546875" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="54" max="54" width="21.85546875" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="55" max="55" width="14.42578125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="56" max="56" width="15.28515625" style="8" customWidth="1"/>
-    <col min="57" max="57" width="14.140625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="58" max="58" width="9.42578125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="60" width="12.42578125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="61" max="61" width="11.42578125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="62" max="62" width="12.42578125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="63" max="63" width="15.28515625" style="8" customWidth="1"/>
-    <col min="64" max="64" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="65" max="65" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="67" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="69" max="69" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="46.25" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="13.25" style="8" customWidth="1"/>
+    <col min="6" max="6" width="21.875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="21.875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="15.25" style="8" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="13" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="15.25" style="8" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="9.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="20" width="12.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="11.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="12.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="15.625" style="8" customWidth="1"/>
+    <col min="24" max="24" width="12.25" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="17.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.75" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="15.875" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="21.875" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="14.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="15.25" style="8" customWidth="1"/>
+    <col min="31" max="31" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="34" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="37" max="37" width="15.25" style="8" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="39" max="39" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="41" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="42" max="42" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="43" max="43" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="44" max="44" width="15.625" style="8" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="46" max="46" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="48" max="48" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="49" max="49" width="15.625" style="8" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="12.25" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="51" max="51" width="17.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.75" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="53" max="53" width="15.875" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="54" max="54" width="21.875" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="55" max="55" width="14.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="56" max="56" width="15.25" style="8" customWidth="1"/>
+    <col min="57" max="57" width="14.125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="58" max="58" width="9.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="60" width="12.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="61" max="61" width="11.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="12.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="63" max="63" width="15.25" style="8" customWidth="1"/>
+    <col min="64" max="64" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="65" max="65" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="67" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="69" max="69" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="70" max="70" width="9" style="8" collapsed="1"/>
     <col min="71" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="I1" s="10" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="I1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10" t="s">
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10" t="s">
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AD1" s="10" t="s">
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AD1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10" t="s">
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10"/>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10"/>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="10" t="s">
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="11"/>
-      <c r="AT1" s="11"/>
-      <c r="AU1" s="11"/>
-      <c r="AV1" s="11"/>
-      <c r="AW1" s="10" t="s">
+      <c r="AS1" s="13"/>
+      <c r="AT1" s="13"/>
+      <c r="AU1" s="13"/>
+      <c r="AV1" s="13"/>
+      <c r="AW1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AX1" s="11"/>
-      <c r="AY1" s="11"/>
-      <c r="AZ1" s="11"/>
-      <c r="BA1" s="11"/>
-      <c r="BD1" s="10" t="s">
+      <c r="AX1" s="13"/>
+      <c r="AY1" s="13"/>
+      <c r="AZ1" s="13"/>
+      <c r="BA1" s="13"/>
+      <c r="BD1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="BE1" s="10"/>
-      <c r="BF1" s="10"/>
-      <c r="BG1" s="10"/>
-      <c r="BH1" s="10"/>
-      <c r="BI1" s="10"/>
-      <c r="BJ1" s="10"/>
-      <c r="BK1" s="10" t="s">
+      <c r="BE1" s="12"/>
+      <c r="BF1" s="12"/>
+      <c r="BG1" s="12"/>
+      <c r="BH1" s="12"/>
+      <c r="BI1" s="12"/>
+      <c r="BJ1" s="12"/>
+      <c r="BK1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="BL1" s="10"/>
-      <c r="BM1" s="10"/>
-      <c r="BN1" s="10"/>
-      <c r="BO1" s="10"/>
-      <c r="BP1" s="10"/>
-      <c r="BQ1" s="10"/>
+      <c r="BL1" s="12"/>
+      <c r="BM1" s="12"/>
+      <c r="BN1" s="12"/>
+      <c r="BO1" s="12"/>
+      <c r="BP1" s="12"/>
+      <c r="BQ1" s="12"/>
     </row>
     <row r="2" spans="1:69" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Uploading the Best buddy results for mcgill university dataset.
</commit_message>
<xml_diff>
--- a/Reports/Thesis/results/Pomeranz 805 Piece Puzzle Results.xlsx
+++ b/Reports/Thesis/results/Pomeranz 805 Piece Puzzle Results.xlsx
@@ -845,6 +845,9 @@
     <xf numFmtId="2" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -852,9 +855,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1287,7 +1287,7 @@
       <c r="E3" s="5">
         <v>97.59</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="11">
         <f t="shared" ref="F3:F21" si="0">100*(1-H3/84)</f>
         <v>94.047619047619051</v>
       </c>
@@ -1315,7 +1315,7 @@
       <c r="E4" s="5">
         <v>99.04</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="11">
         <f t="shared" si="0"/>
         <v>96.428571428571431</v>
       </c>
@@ -1343,7 +1343,7 @@
       <c r="E5" s="5">
         <v>99.77</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="11">
         <f t="shared" si="0"/>
         <v>92.857142857142861</v>
       </c>
@@ -1371,7 +1371,7 @@
       <c r="E6" s="5">
         <v>99.41</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="11">
         <f t="shared" si="0"/>
         <v>88.095238095238088</v>
       </c>
@@ -1399,7 +1399,7 @@
       <c r="E7" s="5">
         <v>96.86</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="11">
         <f t="shared" si="0"/>
         <v>94.047619047619051</v>
       </c>
@@ -1427,7 +1427,7 @@
       <c r="E8" s="5">
         <v>98.59</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="11">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -1455,7 +1455,7 @@
       <c r="E9" s="5">
         <v>99.87</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="11">
         <f t="shared" si="0"/>
         <v>90.476190476190482</v>
       </c>
@@ -1483,7 +1483,7 @@
       <c r="E10" s="5">
         <v>98.57</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="11">
         <f t="shared" si="0"/>
         <v>85.714285714285722</v>
       </c>
@@ -1539,7 +1539,7 @@
       <c r="E12" s="5">
         <v>99.24</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="11">
         <f t="shared" si="0"/>
         <v>95.238095238095227</v>
       </c>
@@ -1567,7 +1567,7 @@
       <c r="E13" s="5">
         <v>97.39</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="11">
         <f t="shared" si="0"/>
         <v>89.285714285714292</v>
       </c>
@@ -1595,7 +1595,7 @@
       <c r="E14" s="5">
         <v>99.29</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="11">
         <f>100*(1-H14/84)</f>
         <v>100</v>
       </c>
@@ -1623,7 +1623,7 @@
       <c r="E15" s="5">
         <v>99.6</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="11">
         <f t="shared" si="0"/>
         <v>90.476190476190482</v>
       </c>
@@ -1651,7 +1651,7 @@
       <c r="E16" s="5">
         <v>98.57</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="11">
         <f t="shared" si="0"/>
         <v>90.476190476190482</v>
       </c>
@@ -1679,7 +1679,7 @@
       <c r="E17" s="5">
         <v>99.38</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="11">
         <f t="shared" si="0"/>
         <v>95.238095238095227</v>
       </c>
@@ -1707,7 +1707,7 @@
       <c r="E18" s="5">
         <v>99.26</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="11">
         <f t="shared" si="0"/>
         <v>92.857142857142861</v>
       </c>
@@ -1735,7 +1735,7 @@
       <c r="E19" s="5">
         <v>98.99</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="11">
         <f t="shared" si="0"/>
         <v>91.666666666666657</v>
       </c>
@@ -1763,7 +1763,7 @@
       <c r="E20" s="5">
         <v>99.8</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="11">
         <f t="shared" si="0"/>
         <v>94.047619047619051</v>
       </c>
@@ -1791,7 +1791,7 @@
       <c r="E21" s="5">
         <v>99.93</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="11">
         <f t="shared" si="0"/>
         <v>86.904761904761912</v>
       </c>
@@ -1812,7 +1812,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1858,115 +1858,195 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="B2" s="3">
+        <v>1682</v>
+      </c>
+      <c r="C2" s="3">
+        <v>97.98</v>
+      </c>
+      <c r="D2" s="3">
+        <v>77.87</v>
+      </c>
+      <c r="E2" s="3">
+        <v>98.62</v>
+      </c>
       <c r="F2" s="9">
         <f>100*(1-H2/94)</f>
-        <v>100</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+        <v>88.297872340425528</v>
+      </c>
+      <c r="G2" s="3">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="B3" s="5">
+        <v>1480</v>
+      </c>
+      <c r="C3" s="5">
+        <v>98.51</v>
+      </c>
+      <c r="D3" s="5">
+        <v>68.52</v>
+      </c>
+      <c r="E3" s="5">
+        <v>98.71</v>
+      </c>
       <c r="F3" s="9">
         <f t="shared" ref="F3:F21" si="0">100*(1-H3/94)</f>
-        <v>100</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+        <v>96.808510638297875</v>
+      </c>
+      <c r="G3" s="5">
+        <v>19</v>
+      </c>
+      <c r="H3" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <f t="shared" ref="A4:A21" si="1">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="B4" s="5">
+        <v>1118</v>
+      </c>
+      <c r="C4" s="5">
+        <v>93.74</v>
+      </c>
+      <c r="D4" s="5">
+        <v>51.76</v>
+      </c>
+      <c r="E4" s="5">
+        <v>94.24</v>
+      </c>
       <c r="F4" s="9">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+        <v>93.61702127659575</v>
+      </c>
+      <c r="G4" s="5">
+        <v>64</v>
+      </c>
+      <c r="H4" s="5">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="B5" s="5">
+        <v>1602</v>
+      </c>
+      <c r="C5" s="5">
+        <v>98.63</v>
+      </c>
+      <c r="D5" s="5">
+        <v>74.17</v>
+      </c>
+      <c r="E5" s="5">
+        <v>98.87</v>
+      </c>
       <c r="F5" s="9">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+        <v>95.744680851063833</v>
+      </c>
+      <c r="G5" s="5">
+        <v>18</v>
+      </c>
+      <c r="H5" s="5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="B6" s="5">
+        <v>1516</v>
+      </c>
+      <c r="C6" s="5">
+        <v>96.97</v>
+      </c>
+      <c r="D6" s="5">
+        <v>70.19</v>
+      </c>
+      <c r="E6" s="5">
+        <v>97.42</v>
+      </c>
       <c r="F6" s="9">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+        <v>92.553191489361694</v>
+      </c>
+      <c r="G6" s="5">
+        <v>39</v>
+      </c>
+      <c r="H6" s="5">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="B7" s="5">
+        <v>1462</v>
+      </c>
+      <c r="C7" s="5">
+        <v>98.5</v>
+      </c>
+      <c r="D7" s="5">
+        <v>67.69</v>
+      </c>
+      <c r="E7" s="5">
+        <v>98.97</v>
+      </c>
       <c r="F7" s="9">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+        <v>92.553191489361694</v>
+      </c>
+      <c r="G7" s="5">
+        <v>15</v>
+      </c>
+      <c r="H7" s="5">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="B8" s="4">
+        <v>1950</v>
+      </c>
+      <c r="C8" s="4">
+        <v>99.69</v>
+      </c>
+      <c r="D8" s="4">
+        <v>90.28</v>
+      </c>
+      <c r="E8" s="4">
+        <v>99.85</v>
+      </c>
       <c r="F8" s="10">
         <f t="shared" si="0"/>
-        <v>94.680851063829792</v>
+        <v>96.808510638297875</v>
       </c>
       <c r="G8" s="4">
         <v>3</v>
       </c>
       <c r="H8" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2030,64 +2110,112 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="B11" s="3">
+        <v>1662</v>
+      </c>
+      <c r="C11" s="3">
+        <v>98.56</v>
+      </c>
+      <c r="D11" s="3">
+        <v>76.94</v>
+      </c>
+      <c r="E11" s="3">
+        <v>99.3</v>
+      </c>
       <c r="F11" s="9">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+        <v>86.170212765957444</v>
+      </c>
+      <c r="G11" s="3">
+        <v>11</v>
+      </c>
+      <c r="H11" s="3">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="B12" s="5">
+        <v>1740</v>
+      </c>
+      <c r="C12" s="5">
+        <v>99.54</v>
+      </c>
+      <c r="D12" s="5">
+        <v>80.56</v>
+      </c>
+      <c r="E12" s="5">
+        <v>99.65</v>
+      </c>
       <c r="F12" s="9">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+        <v>97.872340425531917</v>
+      </c>
+      <c r="G12" s="5">
+        <v>6</v>
+      </c>
+      <c r="H12" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="B13" s="5">
+        <v>1434</v>
+      </c>
+      <c r="C13" s="5">
+        <v>98.19</v>
+      </c>
+      <c r="D13" s="5">
+        <v>66.39</v>
+      </c>
+      <c r="E13" s="5">
+        <v>98.74</v>
+      </c>
       <c r="F13" s="9">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+        <v>91.489361702127653</v>
+      </c>
+      <c r="G13" s="5">
+        <v>18</v>
+      </c>
+      <c r="H13" s="5">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="B14" s="5">
+        <v>1742</v>
+      </c>
+      <c r="C14" s="5">
+        <v>98.74</v>
+      </c>
+      <c r="D14" s="5">
+        <v>80.650000000000006</v>
+      </c>
+      <c r="E14" s="5">
+        <v>99.02</v>
+      </c>
       <c r="F14" s="9">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+        <v>94.680851063829792</v>
+      </c>
+      <c r="G14" s="5">
+        <v>17</v>
+      </c>
+      <c r="H14" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
@@ -2941,36 +3069,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="I1" s="12" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="I1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12" t="s">
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12" t="s">
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
     </row>
     <row r="2" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6486,61 +6614,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="I1" s="12" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="I1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12" t="s">
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12" t="s">
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AD1" s="12" t="s">
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AD1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12" t="s">
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13"/>
+      <c r="AI1" s="13"/>
+      <c r="AJ1" s="13"/>
+      <c r="AK1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12" t="s">
+      <c r="AL1" s="13"/>
+      <c r="AM1" s="13"/>
+      <c r="AN1" s="13"/>
+      <c r="AO1" s="13"/>
+      <c r="AP1" s="13"/>
+      <c r="AQ1" s="13"/>
+      <c r="AR1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="13"/>
-      <c r="AT1" s="13"/>
-      <c r="AU1" s="13"/>
-      <c r="AV1" s="13"/>
+      <c r="AS1" s="14"/>
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="14"/>
     </row>
     <row r="2" spans="1:48" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -13692,86 +13820,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="I1" s="12" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="I1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12" t="s">
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12" t="s">
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AD1" s="12" t="s">
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AD1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12" t="s">
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13"/>
+      <c r="AI1" s="13"/>
+      <c r="AJ1" s="13"/>
+      <c r="AK1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12" t="s">
+      <c r="AL1" s="13"/>
+      <c r="AM1" s="13"/>
+      <c r="AN1" s="13"/>
+      <c r="AO1" s="13"/>
+      <c r="AP1" s="13"/>
+      <c r="AQ1" s="13"/>
+      <c r="AR1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="13"/>
-      <c r="AT1" s="13"/>
-      <c r="AU1" s="13"/>
-      <c r="AV1" s="13"/>
-      <c r="AW1" s="12" t="s">
+      <c r="AS1" s="14"/>
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="14"/>
+      <c r="AW1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AX1" s="13"/>
-      <c r="AY1" s="13"/>
-      <c r="AZ1" s="13"/>
-      <c r="BA1" s="13"/>
-      <c r="BD1" s="12" t="s">
+      <c r="AX1" s="14"/>
+      <c r="AY1" s="14"/>
+      <c r="AZ1" s="14"/>
+      <c r="BA1" s="14"/>
+      <c r="BD1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="BE1" s="12"/>
-      <c r="BF1" s="12"/>
-      <c r="BG1" s="12"/>
-      <c r="BH1" s="12"/>
-      <c r="BI1" s="12"/>
-      <c r="BJ1" s="12"/>
-      <c r="BK1" s="12" t="s">
+      <c r="BE1" s="13"/>
+      <c r="BF1" s="13"/>
+      <c r="BG1" s="13"/>
+      <c r="BH1" s="13"/>
+      <c r="BI1" s="13"/>
+      <c r="BJ1" s="13"/>
+      <c r="BK1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="BL1" s="12"/>
-      <c r="BM1" s="12"/>
-      <c r="BN1" s="12"/>
-      <c r="BO1" s="12"/>
-      <c r="BP1" s="12"/>
-      <c r="BQ1" s="12"/>
+      <c r="BL1" s="13"/>
+      <c r="BM1" s="13"/>
+      <c r="BN1" s="13"/>
+      <c r="BO1" s="13"/>
+      <c r="BP1" s="13"/>
+      <c r="BQ1" s="13"/>
     </row>
     <row r="2" spans="1:69" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">

</xml_diff>